<commit_message>
In pom.xml I added validation dependency. I then updated GoalCreateDto to inject @NotBlank dependency to goal Title, after that I Added a @Valid annotation to createGoal() method. This code make sure Goal Title isn't left null
</commit_message>
<xml_diff>
--- a/Backend/docs/QA-GLPT-test-cases.xlsx
+++ b/Backend/docs/QA-GLPT-test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\IdeaProjects\Global-Legend-Progress-Tracker\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B7FAC7-AAF4-4E31-A1CC-9E2EC96CD5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5947FA-388B-4397-8145-0C3AE16929F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Goal TC-v1.0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="127">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Empty sting is not allowed</t>
   </si>
   <si>
-    <t>Added empty String</t>
-  </si>
-  <si>
     <t>View All Goal</t>
   </si>
   <si>
@@ -451,6 +448,36 @@
   </si>
   <si>
     <t>Return 400 Bad Request</t>
+  </si>
+  <si>
+    <t>Change Log</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Updated TC-G2 status to PASS
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Return error 400</t>
   </si>
 </sst>
 </file>
@@ -525,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -544,12 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -899,14 +920,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D4560-2952-494E-9146-2855A1D08687}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:L20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="77" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
@@ -923,102 +944,110 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="11">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="9">
+        <v>68</v>
+      </c>
+      <c r="B7" s="7">
         <v>45984</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1042,13 +1071,13 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1070,22 +1099,22 @@
         <v>16</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L15" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1093,10 +1122,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -1113,20 +1142,20 @@
       <c r="H16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="7">
+        <v>45985</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L16" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1134,34 +1163,34 @@
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L17" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1169,34 +1198,34 @@
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L18" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1204,192 +1233,192 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="J19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L19" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="8" t="s">
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="J20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L20" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="H21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="I21" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L21" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="J22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L22" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="J23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L23" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1402,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19719A81-4EA2-4DB3-85FF-F2ECC34079C1}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="64" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -1416,108 +1445,108 @@
     <col min="7" max="7" width="22.109375" customWidth="1"/>
     <col min="8" max="8" width="34.44140625" customWidth="1"/>
     <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="11">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="9">
+        <v>68</v>
+      </c>
+      <c r="B7" s="7">
         <v>45984</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1541,355 +1570,355 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L15" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="I16" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L16" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L17" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L18" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="J19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L19" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="J20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L20" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>112</v>
+        <v>117</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="I21" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L21" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="J22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L22" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="7">
+        <v>45984</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L23" s="9">
-        <v>45984</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1906,7 +1935,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1923,7 +1952,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>

</xml_diff>

<commit_message>
Modified GoalService class specifically related to throw exception. Not it succesfully return 400 not found using ResponseStatusException for each method that calls non-existing id
</commit_message>
<xml_diff>
--- a/Backend/docs/QA-GLPT-test-cases.xlsx
+++ b/Backend/docs/QA-GLPT-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\IdeaProjects\Global-Legend-Progress-Tracker\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5947FA-388B-4397-8145-0C3AE16929F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA19DF07-9A50-440E-9665-C1EC15C65D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
   </bookViews>
@@ -176,9 +176,6 @@
 to Master Javascript</t>
   </si>
   <si>
-    <t>Rename an non-exisiting Goal</t>
-  </si>
-  <si>
     <t>http://localhost:8080/goals/999?newTitle=Master Javascript</t>
   </si>
   <si>
@@ -451,6 +448,12 @@
   </si>
   <si>
     <t>Change Log</t>
+  </si>
+  <si>
+    <t>Return error 400</t>
+  </si>
+  <si>
+    <t>Rename a non-exisiting Goal</t>
   </si>
   <si>
     <r>
@@ -462,7 +465,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.1</t>
+      <t>1.0</t>
     </r>
     <r>
       <rPr>
@@ -472,12 +475,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Updated TC-G2 status to PASS
+      <t xml:space="preserve"> 
+ - Updated TC-G2 actual result and status to PASS
+- Updated TC-G5 actual result and status to PASS
+- Updated TC-G7 actual result and status to PASS
+- Updated TC-G9 actual result and status to PASS
 </t>
     </r>
-  </si>
-  <si>
-    <t>Return error 400</t>
   </si>
 </sst>
 </file>
@@ -920,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D4560-2952-494E-9146-2855A1D08687}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="77" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,47 +948,47 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
@@ -992,7 +996,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="7">
         <v>45984</v>
@@ -1000,42 +1004,42 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1044,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1071,13 +1075,13 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1105,16 +1109,16 @@
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15" s="7">
         <v>45984</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1122,10 +1126,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -1143,19 +1147,19 @@
         <v>20</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L16" s="7">
         <v>45985</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1181,16 +1185,16 @@
         <v>17</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L17" s="7">
         <v>45984</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1216,16 +1220,16 @@
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L18" s="7">
         <v>45984</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1233,10 +1237,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>26</v>
@@ -1253,20 +1257,20 @@
       <c r="H19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="6" t="s">
+      <c r="I19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="7">
+        <v>45985</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="L19" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1280,7 +1284,7 @@
         <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>38</v>
@@ -1292,16 +1296,16 @@
         <v>39</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L20" s="7">
         <v>45984</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1309,95 +1313,95 @@
         <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="I21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="7">
+        <v>45985</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="L21" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="J22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="7">
         <v>45984</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>31</v>
@@ -1405,20 +1409,20 @@
       <c r="H23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="6" t="s">
+      <c r="I23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="7">
+        <v>45985</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="L23" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1451,47 +1455,47 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
@@ -1499,7 +1503,7 @@
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="7">
         <v>45984</v>
@@ -1507,34 +1511,34 @@
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1543,10 +1547,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1570,73 +1574,73 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15" s="7">
         <v>45984</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>33</v>
@@ -1645,185 +1649,185 @@
         <v>32</v>
       </c>
       <c r="J16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="L16" s="7">
         <v>45984</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L17" s="7">
         <v>45984</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L18" s="7">
         <v>45984</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L19" s="7">
         <v>45984</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L20" s="7">
         <v>45984</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>33</v>
@@ -1832,93 +1836,93 @@
         <v>32</v>
       </c>
       <c r="J21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="L21" s="7">
         <v>45984</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="J22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="7">
         <v>45984</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L23" s="7">
         <v>45984</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1952,7 +1956,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>

</xml_diff>

<commit_message>
Updated my test cases and alll succesfully pass. Updated ProgressEntryService and modified throw exception to ResponseStatuseException. It now succesfully return error 400 instead of 500
</commit_message>
<xml_diff>
--- a/Backend/docs/QA-GLPT-test-cases.xlsx
+++ b/Backend/docs/QA-GLPT-test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\IdeaProjects\Global-Legend-Progress-Tracker\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA19DF07-9A50-440E-9665-C1EC15C65D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6222B96E-722E-4F5A-BCE2-19C4480136BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Goal TC-v1.0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -147,10 +147,6 @@
     <t xml:space="preserve"> http://localhost:8080/goals/999</t>
   </si>
   <si>
-    <t>Return 500 Internal 
-Server error</t>
-  </si>
-  <si>
     <t>Error 404 no Id found</t>
   </si>
   <si>
@@ -218,9 +214,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Rustom</t>
   </si>
   <si>
@@ -442,9 +435,6 @@
   </si>
   <si>
     <t>Delete a non-exisiting Entry</t>
-  </si>
-  <si>
-    <t>Return 400 Bad Request</t>
   </si>
   <si>
     <t>Change Log</t>
@@ -482,6 +472,40 @@
 - Updated TC-G9 actual result and status to PASS
 </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1.0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ - Updated TC-E2 actual result and status to PASS
+-  Updated TC-E7 actual result and status to PASS
+- Updated TC-E9 actual result and status to PASS
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Need to think about this one.
+- Do user need empty entry?</t>
   </si>
 </sst>
 </file>
@@ -533,13 +557,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -573,9 +597,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -585,7 +606,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -924,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D4560-2952-494E-9146-2855A1D08687}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="77" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView topLeftCell="A19" zoomScale="77" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,110 +975,110 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>76</v>
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="9">
+        <v>64</v>
+      </c>
+      <c r="B6" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="7">
+        <v>65</v>
+      </c>
+      <c r="B7" s="6">
         <v>45984</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>76</v>
+        <v>66</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="13" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1075,13 +1102,13 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1109,16 +1136,16 @@
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <v>45984</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1126,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -1147,19 +1174,19 @@
         <v>20</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>45985</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1170,7 +1197,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
@@ -1185,16 +1212,16 @@
         <v>17</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>45984</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1205,7 +1232,7 @@
         <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>30</v>
@@ -1220,16 +1247,16 @@
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>45984</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -1237,16 +1264,16 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>30</v>
@@ -1255,174 +1282,174 @@
         <v>31</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="L19" s="6">
         <v>45985</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="J20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="7">
+      <c r="L20" s="6">
         <v>45984</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L21" s="7">
+      <c r="L21" s="6">
         <v>45985</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="7">
+      <c r="L22" s="6">
         <v>45984</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L23" s="7">
+      <c r="L23" s="6">
         <v>45985</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1433,16 +1460,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19719A81-4EA2-4DB3-85FF-F2ECC34079C1}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="64" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="64" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
@@ -1451,106 +1478,115 @@
     <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="6" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="8" t="s">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="7">
-        <v>45984</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -1574,355 +1610,363 @@
         <v>7</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N14" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <v>45984</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="I16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="6">
+        <v>45985</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="I17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="J17" s="11"/>
       <c r="K17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17" s="7">
+        <v>53</v>
+      </c>
+      <c r="L17" s="6">
         <v>45984</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>45984</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="J19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="L19" s="6">
         <v>45984</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="6">
+        <v>45984</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="E21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="L21" s="6">
+        <v>45985</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L21" s="7">
-        <v>45984</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="J22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="7">
+      <c r="L22" s="6">
         <v>45984</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J23" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="K23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L23" s="7">
-        <v>45984</v>
+        <v>53</v>
+      </c>
+      <c r="L23" s="6">
+        <v>45985</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1937,9 +1981,9 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1954,9 +1998,9 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>

</xml_diff>

<commit_message>
Updated Goal Entity Class for entries List. Added cascadeTpe remove and orphanRemoval. This make sure the goal is deleted with it's entries. There were two options to solve goal deletion either cascading from field entity or updating deleteGoal method to manually delete entries and goal.
</commit_message>
<xml_diff>
--- a/Backend/docs/QA-GLPT-test-cases.xlsx
+++ b/Backend/docs/QA-GLPT-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\IdeaProjects\Global-Legend-Progress-Tracker\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6222B96E-722E-4F5A-BCE2-19C4480136BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C62CBEC-DBAD-43D6-829C-6D2DC1270B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -506,6 +506,18 @@
   <si>
     <t>Need to think about this one.
 - Do user need empty entry?</t>
+  </si>
+  <si>
+    <t>TC-G10</t>
+  </si>
+  <si>
+    <t>Delete an existing Goal with entry/entries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://localhost:8080/goals/3</t>
+  </si>
+  <si>
+    <t>Resolve</t>
   </si>
 </sst>
 </file>
@@ -580,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -614,6 +626,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D4560-2952-494E-9146-2855A1D08687}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="77" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,6 +998,9 @@
       <c r="B1" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="C1" s="13" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -988,6 +1009,9 @@
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="C2" s="13">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -996,6 +1020,7 @@
       <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1449,6 +1474,47 @@
         <v>45985</v>
       </c>
       <c r="M23" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="6">
+        <v>45986</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1462,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19719A81-4EA2-4DB3-85FF-F2ECC34079C1}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="64" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1488,6 +1554,9 @@
       <c r="B1" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="C1" s="13" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1495,6 +1564,9 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>78</v>
+      </c>
+      <c r="C2" s="13">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated test case for deleting goal with entry
</commit_message>
<xml_diff>
--- a/Backend/docs/QA-GLPT-test-cases.xlsx
+++ b/Backend/docs/QA-GLPT-test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\IdeaProjects\Global-Legend-Progress-Tracker\Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C62CBEC-DBAD-43D6-829C-6D2DC1270B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C83AA4-5775-4047-AC32-5304DF2D472A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D0027813-B7E4-45FD-BDF3-ECB36AA97A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Goal TC-v1.0" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>Resolve</t>
+  </si>
+  <si>
+    <t>Very Crucial as it wasn't able to delete because it has a relationship with another table</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -625,9 +628,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -967,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84D4560-2952-494E-9146-2855A1D08687}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="54" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,41 +988,41 @@
     <col min="11" max="11" width="8.88671875" style="3"/>
     <col min="12" max="12" width="12.109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="14" max="14" width="32.109375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>62</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>45984</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>120</v>
       </c>
@@ -1094,8 +1094,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -1135,8 +1135,11 @@
       <c r="M14" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N14" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>127</v>
       </c>
@@ -1516,6 +1519,9 @@
       </c>
       <c r="M24" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1528,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19719A81-4EA2-4DB3-85FF-F2ECC34079C1}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A12" zoomScale="64" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1554,7 +1560,7 @@
       <c r="B1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1565,7 +1571,7 @@
       <c r="B2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>3</v>
       </c>
     </row>

</xml_diff>